<commit_message>
fix: WorklogSealing pouchDepth 타입을 decimal로 변경 및 DTO 필드명 엔티티와 동기화
</commit_message>
<xml_diff>
--- a/data/templates/worklog/11.Sealing.xlsx
+++ b/data/templates/worklog/11.Sealing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\eurocell-mes-be\data\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\eurocell-mes-be\data\templates\worklog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB3ABD5-1253-4940-B2D3-6F00F7BC1ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC55D121-6FDD-4A6C-B1D1-02E86BB9D259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17085" yWindow="75" windowWidth="19140" windowHeight="15210" xr2:uid="{4D09F8EE-03B8-4266-9ABE-BF29521CAAED}"/>
+    <workbookView xWindow="720" yWindow="1425" windowWidth="24705" windowHeight="13965" xr2:uid="{4D09F8EE-03B8-4266-9ABE-BF29521CAAED}"/>
   </bookViews>
   <sheets>
     <sheet name="원본" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,8 @@
     <definedName name="hipot3GoodQuantity">원본!$G$23</definedName>
     <definedName name="hipot3JrNumber">원본!$C$23</definedName>
     <definedName name="hipot3WorkQuantity">원본!$E$23</definedName>
+    <definedName name="hipotTime">원본!$E$35</definedName>
+    <definedName name="hipotVoltage">원본!$C$35</definedName>
     <definedName name="jigNumber">원본!$G$37</definedName>
     <definedName name="line">원본!$C$9</definedName>
     <definedName name="manufactureDate">원본!$C$7</definedName>

</xml_diff>